<commit_message>
Added Test Cases: 1)Adding, Updating and Deleting Language 2)Testing the Language Feature 3)Testing the Description Feature
</commit_message>
<xml_diff>
--- a/MarsQA-1/SpecflowTests/Data/Data.xlsx
+++ b/MarsQA-1/SpecflowTests/Data/Data.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{682964AA-AE86-4345-A280-B3C857B03A25}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-24030" yWindow="-2895" windowWidth="20460" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Language" sheetId="1" r:id="rId1"/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Language</t>
   </si>
@@ -35,12 +36,15 @@
   </si>
   <si>
     <t>Korean</t>
+  </si>
+  <si>
+    <t>Filipino</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -166,6 +170,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -201,6 +222,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -376,11 +414,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -417,6 +455,11 @@
         <v>6</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>

</xml_diff>